<commit_message>
Retrospective and Backlog of week 7
</commit_message>
<xml_diff>
--- a/doc/Scrum/Backlogs/Backlog week 6.xlsx
+++ b/doc/Scrum/Backlogs/Backlog week 6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\template\doc\Scrum\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{669F024D-E9AC-4FCF-BFC2-41F24CB3F4D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE0F9BE-9F3B-494F-82BD-2B60CFE75A39}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{756426E5-5797-4A5B-B234-946B539A862C}"/>
+    <workbookView minimized="1" xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="8964" xr2:uid="{756426E5-5797-4A5B-B234-946B539A862C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07C6E92-69A2-4827-8299-B8E61DF34548}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>

</xml_diff>